<commit_message>
Changes to addiction definition
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Intervention_Defs.xlsx
+++ b/inputs/AddictO_Intervention_Defs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="526">
   <si>
     <t>ID</t>
   </si>
@@ -1597,6 +1597,15 @@
   </si>
   <si>
     <t xml:space="preserve">No ontological definition found. </t>
+  </si>
+  <si>
+    <t>Treatment success</t>
+  </si>
+  <si>
+    <t>A treatment outcome in which the aims of the treatment have been achieved.</t>
+  </si>
+  <si>
+    <t>Treatment outcome</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1810,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2099,11 +2108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S339"/>
+  <dimension ref="A1:S340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C235" sqref="C235"/>
+      <pane ySplit="1" topLeftCell="A295" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8254,31 +8263,39 @@
       </c>
       <c r="R307" s="12"/>
     </row>
-    <row r="308" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A308" s="12"/>
       <c r="B308" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="C308" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="D308" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="E308" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F308" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R308" s="12"/>
+    </row>
+    <row r="309" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B309" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="F308" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P308" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="309" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B309" s="13" t="s">
+      <c r="F309" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P309" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="310" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B310" s="13" t="s">
         <v>270</v>
-      </c>
-      <c r="F309" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P309" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="310" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B310" s="13" t="s">
-        <v>271</v>
       </c>
       <c r="F310" s="11" t="s">
         <v>5</v>
@@ -8289,32 +8306,32 @@
     </row>
     <row r="311" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B311" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F311" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P311" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="312" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B312" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="F311" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I311" s="11" t="s">
+      <c r="F312" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I312" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="P311" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="312" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B312" s="11" t="s">
+      <c r="P312" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="313" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B313" s="11" t="s">
         <v>470</v>
-      </c>
-      <c r="F312" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P312" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="313" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B313" s="11" t="s">
-        <v>471</v>
       </c>
       <c r="F313" s="11" t="s">
         <v>5</v>
@@ -8325,43 +8342,48 @@
     </row>
     <row r="314" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B314" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="F314" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P314" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="315" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B315" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="F314" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P314" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q314" s="13"/>
-    </row>
-    <row r="315" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B315" s="14"/>
+      <c r="F315" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="P315" s="11" t="s">
         <v>155</v>
       </c>
+      <c r="Q315" s="13"/>
     </row>
     <row r="316" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B316" s="14"/>
-      <c r="F316" s="12"/>
-      <c r="G316" s="12"/>
-      <c r="H316" s="14"/>
-      <c r="I316" s="12"/>
-      <c r="J316" s="12"/>
-      <c r="K316" s="12"/>
-      <c r="L316" s="12">
-        <v>1</v>
-      </c>
-      <c r="M316" s="12"/>
-      <c r="N316" s="12"/>
-      <c r="O316" s="12"/>
-      <c r="P316" s="12"/>
+      <c r="P316" s="11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="317" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B317" s="14"/>
-      <c r="P317" s="11" t="s">
-        <v>155</v>
-      </c>
+      <c r="F317" s="12"/>
+      <c r="G317" s="12"/>
+      <c r="H317" s="14"/>
+      <c r="I317" s="12"/>
+      <c r="J317" s="12"/>
+      <c r="K317" s="12"/>
+      <c r="L317" s="12">
+        <v>1</v>
+      </c>
+      <c r="M317" s="12"/>
+      <c r="N317" s="12"/>
+      <c r="O317" s="12"/>
+      <c r="P317" s="12"/>
     </row>
     <row r="318" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B318" s="14"/>
@@ -8377,42 +8399,31 @@
     </row>
     <row r="320" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B320" s="14"/>
-      <c r="D320" s="12"/>
-      <c r="E320" s="12"/>
-      <c r="F320" s="12"/>
-      <c r="G320" s="12"/>
-      <c r="H320" s="12"/>
-      <c r="I320" s="12"/>
-      <c r="J320" s="12"/>
-      <c r="K320" s="12"/>
-      <c r="L320" s="12"/>
-      <c r="M320" s="12"/>
-      <c r="N320" s="12"/>
-      <c r="O320" s="12"/>
-      <c r="P320" s="12"/>
+      <c r="P320" s="11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="321" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B321" s="14"/>
-      <c r="P321" s="11" t="s">
-        <v>155</v>
-      </c>
+      <c r="D321" s="12"/>
+      <c r="E321" s="12"/>
+      <c r="F321" s="12"/>
+      <c r="G321" s="12"/>
+      <c r="H321" s="12"/>
+      <c r="I321" s="12"/>
+      <c r="J321" s="12"/>
+      <c r="K321" s="12"/>
+      <c r="L321" s="12"/>
+      <c r="M321" s="12"/>
+      <c r="N321" s="12"/>
+      <c r="O321" s="12"/>
+      <c r="P321" s="12"/>
     </row>
     <row r="322" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B322" s="14"/>
-      <c r="C322" s="12"/>
-      <c r="D322" s="12"/>
-      <c r="E322" s="12"/>
-      <c r="F322" s="12"/>
-      <c r="G322" s="12"/>
-      <c r="H322" s="12"/>
-      <c r="I322" s="12"/>
-      <c r="J322" s="12"/>
-      <c r="K322" s="12"/>
-      <c r="L322" s="12"/>
-      <c r="M322" s="12"/>
-      <c r="N322" s="12"/>
-      <c r="O322" s="12"/>
-      <c r="P322" s="12"/>
+      <c r="P322" s="11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="323" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B323" s="14"/>
@@ -8433,10 +8444,24 @@
     </row>
     <row r="324" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B324" s="14"/>
-      <c r="Q324" s="12"/>
+      <c r="C324" s="12"/>
+      <c r="D324" s="12"/>
+      <c r="E324" s="12"/>
+      <c r="F324" s="12"/>
+      <c r="G324" s="12"/>
+      <c r="H324" s="12"/>
+      <c r="I324" s="12"/>
+      <c r="J324" s="12"/>
+      <c r="K324" s="12"/>
+      <c r="L324" s="12"/>
+      <c r="M324" s="12"/>
+      <c r="N324" s="12"/>
+      <c r="O324" s="12"/>
+      <c r="P324" s="12"/>
     </row>
     <row r="325" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B325" s="14"/>
+      <c r="Q325" s="12"/>
     </row>
     <row r="326" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B326" s="14"/>
@@ -8460,30 +8485,16 @@
       <c r="B332" s="14"/>
     </row>
     <row r="333" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A333" s="14"/>
       <c r="B333" s="14"/>
-      <c r="R333" s="12"/>
     </row>
     <row r="334" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="14"/>
       <c r="B334" s="14"/>
-      <c r="Q334" s="12"/>
+      <c r="R334" s="12"/>
     </row>
     <row r="335" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B335" s="14"/>
-      <c r="C335" s="12"/>
-      <c r="D335" s="12"/>
-      <c r="E335" s="12"/>
-      <c r="F335" s="12"/>
-      <c r="G335" s="12"/>
-      <c r="H335" s="12"/>
-      <c r="I335" s="12"/>
-      <c r="J335" s="12"/>
-      <c r="K335" s="12"/>
-      <c r="L335" s="12"/>
-      <c r="M335" s="12"/>
-      <c r="N335" s="12"/>
-      <c r="O335" s="12"/>
-      <c r="P335" s="12"/>
+      <c r="Q335" s="12"/>
     </row>
     <row r="336" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B336" s="14"/>
@@ -8501,10 +8512,8 @@
       <c r="N336" s="12"/>
       <c r="O336" s="12"/>
       <c r="P336" s="12"/>
-      <c r="Q336" s="12"/>
     </row>
     <row r="337" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="12"/>
       <c r="B337" s="14"/>
       <c r="C337" s="12"/>
       <c r="D337" s="12"/>
@@ -8521,9 +8530,9 @@
       <c r="O337" s="12"/>
       <c r="P337" s="12"/>
       <c r="Q337" s="12"/>
-      <c r="R337" s="12"/>
     </row>
     <row r="338" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="12"/>
       <c r="B338" s="14"/>
       <c r="C338" s="12"/>
       <c r="D338" s="12"/>
@@ -8540,9 +8549,28 @@
       <c r="O338" s="12"/>
       <c r="P338" s="12"/>
       <c r="Q338" s="12"/>
-    </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R338" s="12"/>
+    </row>
+    <row r="339" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B339" s="14"/>
+      <c r="C339" s="12"/>
+      <c r="D339" s="12"/>
+      <c r="E339" s="12"/>
+      <c r="F339" s="12"/>
+      <c r="G339" s="12"/>
+      <c r="H339" s="12"/>
+      <c r="I339" s="12"/>
+      <c r="J339" s="12"/>
+      <c r="K339" s="12"/>
+      <c r="L339" s="12"/>
+      <c r="M339" s="12"/>
+      <c r="N339" s="12"/>
+      <c r="O339" s="12"/>
+      <c r="P339" s="12"/>
+      <c r="Q339" s="12"/>
+    </row>
+    <row r="340" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B340" s="14"/>
     </row>
   </sheetData>
   <sortState ref="A2:S2822">

</xml_diff>

<commit_message>
Removed some entries that were out of scope
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Intervention_Defs.xlsx
+++ b/inputs/AddictO_Intervention_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharoncox/Documents/GitHub/addiction-ontology/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFC81E4-7F36-8D4B-A6B7-E1CDE62E1835}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FC22D-5241-2F43-AEF6-B3A38FC1AF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10740" yWindow="5080" windowWidth="14260" windowHeight="9940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="529">
   <si>
     <t>ID</t>
   </si>
@@ -1610,6 +1610,12 @@
   </si>
   <si>
     <t>TV advertising</t>
+  </si>
+  <si>
+    <t>Advertising</t>
+  </si>
+  <si>
+    <t>Radio advertising</t>
   </si>
 </sst>
 </file>
@@ -2112,11 +2118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T341"/>
+  <dimension ref="A1:T342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A309" sqref="A309:XFD309"/>
+      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B310" sqref="B310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8305,20 +8311,28 @@
       </c>
       <c r="T309" s="15"/>
     </row>
-    <row r="310" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B310" s="11" t="s">
+    <row r="310" spans="1:20" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B310" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="D310" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="H310" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L310" s="15"/>
+      <c r="P310" s="17">
+        <v>1</v>
+      </c>
+      <c r="R310" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="T310" s="15"/>
+    </row>
+    <row r="311" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B311" s="11" t="s">
         <v>465</v>
-      </c>
-      <c r="F310" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P310" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="311" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B311" s="13" t="s">
-        <v>269</v>
       </c>
       <c r="F311" s="11" t="s">
         <v>5</v>
@@ -8329,7 +8343,7 @@
     </row>
     <row r="312" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B312" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F312" s="11" t="s">
         <v>5</v>
@@ -8340,79 +8354,84 @@
     </row>
     <row r="313" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B313" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="F313" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P313" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="314" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B314" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="F313" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I313" s="11" t="s">
+      <c r="F314" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I314" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="P313" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="314" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B314" s="11" t="s">
+      <c r="P314" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="315" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B315" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="F314" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P314" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="315" spans="1:20" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="B315" s="11" t="s">
+      <c r="F315" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P315" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="316" spans="1:20" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B316" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="F315" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P315" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="316" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B316" s="11" t="s">
+      <c r="F316" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P316" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="317" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B317" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="F316" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P316" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q316" s="13"/>
-    </row>
-    <row r="317" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B317" s="14"/>
+      <c r="F317" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="P317" s="11" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="318" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q317" s="13"/>
+    </row>
+    <row r="318" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B318" s="14"/>
-      <c r="F318" s="12"/>
-      <c r="G318" s="12"/>
-      <c r="H318" s="14"/>
-      <c r="I318" s="12"/>
-      <c r="J318" s="12"/>
-      <c r="K318" s="12"/>
-      <c r="L318" s="12">
-        <v>1</v>
-      </c>
-      <c r="M318" s="12"/>
-      <c r="N318" s="12"/>
-      <c r="O318" s="12"/>
-      <c r="P318" s="12"/>
-    </row>
-    <row r="319" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="P318" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="319" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B319" s="14"/>
-      <c r="P319" s="11" t="s">
-        <v>154</v>
-      </c>
+      <c r="F319" s="12"/>
+      <c r="G319" s="12"/>
+      <c r="H319" s="14"/>
+      <c r="I319" s="12"/>
+      <c r="J319" s="12"/>
+      <c r="K319" s="12"/>
+      <c r="L319" s="12">
+        <v>1</v>
+      </c>
+      <c r="M319" s="12"/>
+      <c r="N319" s="12"/>
+      <c r="O319" s="12"/>
+      <c r="P319" s="12"/>
     </row>
     <row r="320" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B320" s="14"/>
@@ -8426,44 +8445,33 @@
         <v>154</v>
       </c>
     </row>
-    <row r="322" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B322" s="14"/>
-      <c r="D322" s="12"/>
-      <c r="E322" s="12"/>
-      <c r="F322" s="12"/>
-      <c r="G322" s="12"/>
-      <c r="H322" s="12"/>
-      <c r="I322" s="12"/>
-      <c r="J322" s="12"/>
-      <c r="K322" s="12"/>
-      <c r="L322" s="12"/>
-      <c r="M322" s="12"/>
-      <c r="N322" s="12"/>
-      <c r="O322" s="12"/>
-      <c r="P322" s="12"/>
-    </row>
-    <row r="323" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="P322" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="323" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B323" s="14"/>
-      <c r="P323" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="324" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D323" s="12"/>
+      <c r="E323" s="12"/>
+      <c r="F323" s="12"/>
+      <c r="G323" s="12"/>
+      <c r="H323" s="12"/>
+      <c r="I323" s="12"/>
+      <c r="J323" s="12"/>
+      <c r="K323" s="12"/>
+      <c r="L323" s="12"/>
+      <c r="M323" s="12"/>
+      <c r="N323" s="12"/>
+      <c r="O323" s="12"/>
+      <c r="P323" s="12"/>
+    </row>
+    <row r="324" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B324" s="14"/>
-      <c r="C324" s="12"/>
-      <c r="D324" s="12"/>
-      <c r="E324" s="12"/>
-      <c r="F324" s="12"/>
-      <c r="G324" s="12"/>
-      <c r="H324" s="12"/>
-      <c r="I324" s="12"/>
-      <c r="J324" s="12"/>
-      <c r="K324" s="12"/>
-      <c r="L324" s="12"/>
-      <c r="M324" s="12"/>
-      <c r="N324" s="12"/>
-      <c r="O324" s="12"/>
-      <c r="P324" s="12"/>
+      <c r="P324" s="11" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="325" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B325" s="14"/>
@@ -8484,10 +8492,24 @@
     </row>
     <row r="326" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B326" s="14"/>
-      <c r="Q326" s="12"/>
+      <c r="C326" s="12"/>
+      <c r="D326" s="12"/>
+      <c r="E326" s="12"/>
+      <c r="F326" s="12"/>
+      <c r="G326" s="12"/>
+      <c r="H326" s="12"/>
+      <c r="I326" s="12"/>
+      <c r="J326" s="12"/>
+      <c r="K326" s="12"/>
+      <c r="L326" s="12"/>
+      <c r="M326" s="12"/>
+      <c r="N326" s="12"/>
+      <c r="O326" s="12"/>
+      <c r="P326" s="12"/>
     </row>
     <row r="327" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B327" s="14"/>
+      <c r="Q327" s="12"/>
     </row>
     <row r="328" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B328" s="14"/>
@@ -8511,30 +8533,16 @@
       <c r="B334" s="14"/>
     </row>
     <row r="335" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="14"/>
       <c r="B335" s="14"/>
-      <c r="R335" s="12"/>
     </row>
     <row r="336" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="14"/>
       <c r="B336" s="14"/>
-      <c r="Q336" s="12"/>
+      <c r="R336" s="12"/>
     </row>
     <row r="337" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B337" s="14"/>
-      <c r="C337" s="12"/>
-      <c r="D337" s="12"/>
-      <c r="E337" s="12"/>
-      <c r="F337" s="12"/>
-      <c r="G337" s="12"/>
-      <c r="H337" s="12"/>
-      <c r="I337" s="12"/>
-      <c r="J337" s="12"/>
-      <c r="K337" s="12"/>
-      <c r="L337" s="12"/>
-      <c r="M337" s="12"/>
-      <c r="N337" s="12"/>
-      <c r="O337" s="12"/>
-      <c r="P337" s="12"/>
+      <c r="Q337" s="12"/>
     </row>
     <row r="338" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B338" s="14"/>
@@ -8552,10 +8560,8 @@
       <c r="N338" s="12"/>
       <c r="O338" s="12"/>
       <c r="P338" s="12"/>
-      <c r="Q338" s="12"/>
     </row>
     <row r="339" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A339" s="12"/>
       <c r="B339" s="14"/>
       <c r="C339" s="12"/>
       <c r="D339" s="12"/>
@@ -8572,9 +8578,9 @@
       <c r="O339" s="12"/>
       <c r="P339" s="12"/>
       <c r="Q339" s="12"/>
-      <c r="R339" s="12"/>
     </row>
     <row r="340" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="12"/>
       <c r="B340" s="14"/>
       <c r="C340" s="12"/>
       <c r="D340" s="12"/>
@@ -8591,15 +8597,34 @@
       <c r="O340" s="12"/>
       <c r="P340" s="12"/>
       <c r="Q340" s="12"/>
-    </row>
-    <row r="341" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R340" s="12"/>
+    </row>
+    <row r="341" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B341" s="14"/>
+      <c r="C341" s="12"/>
+      <c r="D341" s="12"/>
+      <c r="E341" s="12"/>
+      <c r="F341" s="12"/>
+      <c r="G341" s="12"/>
+      <c r="H341" s="12"/>
+      <c r="I341" s="12"/>
+      <c r="J341" s="12"/>
+      <c r="K341" s="12"/>
+      <c r="L341" s="12"/>
+      <c r="M341" s="12"/>
+      <c r="N341" s="12"/>
+      <c r="O341" s="12"/>
+      <c r="P341" s="12"/>
+      <c r="Q341" s="12"/>
+    </row>
+    <row r="342" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B342" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="A2:S2823">
-    <sortCondition ref="F2:F2823"/>
-    <sortCondition descending="1" ref="N2:N2823"/>
-    <sortCondition ref="B2:B2823"/>
+  <sortState ref="A2:S2824">
+    <sortCondition ref="F2:F2824"/>
+    <sortCondition descending="1" ref="N2:N2824"/>
+    <sortCondition ref="B2:B2824"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="G179" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Discussion 14 May 2020
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Intervention_Defs.xlsx
+++ b/inputs/AddictO_Intervention_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FC22D-5241-2F43-AEF6-B3A38FC1AF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB0DA97-C9F1-4195-8CED-12625B1F8E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="5080" windowWidth="14260" windowHeight="9940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="530">
   <si>
     <t>ID</t>
   </si>
@@ -1616,13 +1616,16 @@
   </si>
   <si>
     <t>Radio advertising</t>
+  </si>
+  <si>
+    <t>An action specification that an organisation produces that includes rules and regulations concerning activities of agents under the organisation's jurisdiction.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1700,6 +1703,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1722,7 +1732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1781,6 +1791,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2121,34 +2140,34 @@
   <dimension ref="A1:T342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B310" sqref="B310"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.5" style="12" customWidth="1"/>
-    <col min="3" max="3" width="64.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="64.453125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="16" style="12" customWidth="1"/>
-    <col min="7" max="7" width="35.5" style="12" customWidth="1"/>
-    <col min="8" max="8" width="48.33203125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="12" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="44.1640625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="12"/>
-    <col min="13" max="13" width="18.5" style="12" customWidth="1"/>
-    <col min="14" max="15" width="9.1640625" style="12"/>
-    <col min="16" max="16" width="13.5" style="12" customWidth="1"/>
-    <col min="17" max="17" width="37.1640625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="48.6640625" style="12" customWidth="1"/>
-    <col min="19" max="19" width="24.6640625" style="12" customWidth="1"/>
-    <col min="20" max="16384" width="9.1640625" style="12"/>
+    <col min="7" max="7" width="35.453125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="48.36328125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="29.6328125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="44.1796875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="12"/>
+    <col min="13" max="13" width="18.453125" style="12" customWidth="1"/>
+    <col min="14" max="15" width="9.1796875" style="12"/>
+    <col min="16" max="16" width="13.453125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="37.1796875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="48.6328125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="24.6328125" style="12" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2204,7 +2223,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>155</v>
       </c>
@@ -2230,7 +2249,7 @@
       </c>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>156</v>
       </c>
@@ -2256,7 +2275,7 @@
       </c>
       <c r="S3" s="13"/>
     </row>
-    <row r="4" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>157</v>
       </c>
@@ -2284,7 +2303,7 @@
       </c>
       <c r="S4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>159</v>
       </c>
@@ -2310,7 +2329,7 @@
       </c>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>160</v>
       </c>
@@ -2336,7 +2355,7 @@
       </c>
       <c r="S6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>161</v>
       </c>
@@ -2364,7 +2383,7 @@
       </c>
       <c r="S7" s="13"/>
     </row>
-    <row r="8" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="13" t="s">
         <v>163</v>
@@ -2393,7 +2412,7 @@
       <c r="R8" s="14"/>
       <c r="S8" s="13"/>
     </row>
-    <row r="9" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>164</v>
       </c>
@@ -2418,7 +2437,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
         <v>165</v>
@@ -2446,7 +2465,7 @@
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>166</v>
       </c>
@@ -2471,7 +2490,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>167</v>
       </c>
@@ -2496,7 +2515,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13" t="s">
         <v>168</v>
@@ -2524,7 +2543,7 @@
       <c r="Q13" s="13"/>
       <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="13" t="s">
         <v>169</v>
@@ -2552,7 +2571,7 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="14"/>
     </row>
-    <row r="15" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>170</v>
       </c>
@@ -2577,7 +2596,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
         <v>171</v>
@@ -2605,7 +2624,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="14"/>
     </row>
-    <row r="17" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>172</v>
       </c>
@@ -2630,7 +2649,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13" t="s">
         <v>173</v>
@@ -2658,7 +2677,7 @@
       <c r="Q18" s="13"/>
       <c r="R18" s="14"/>
     </row>
-    <row r="19" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
         <v>174</v>
       </c>
@@ -2683,7 +2702,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
         <v>175</v>
@@ -2711,7 +2730,7 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="14"/>
     </row>
-    <row r="21" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="13" t="s">
         <v>176</v>
       </c>
@@ -2736,7 +2755,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>177</v>
       </c>
@@ -2761,7 +2780,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
         <v>178</v>
@@ -2789,7 +2808,7 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="14"/>
     </row>
-    <row r="24" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
         <v>179</v>
@@ -2817,7 +2836,7 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="14"/>
     </row>
-    <row r="25" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13" t="s">
         <v>180</v>
@@ -2845,7 +2864,7 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="14"/>
     </row>
-    <row r="26" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="13" t="s">
         <v>181</v>
@@ -2873,7 +2892,7 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="14"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
         <v>182</v>
       </c>
@@ -2898,7 +2917,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="13" t="s">
         <v>183</v>
       </c>
@@ -2923,7 +2942,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13" t="s">
         <v>184</v>
@@ -2951,7 +2970,7 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="14"/>
     </row>
-    <row r="30" spans="1:18" s="11" customFormat="1" ht="208" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="11" customFormat="1" ht="203" x14ac:dyDescent="0.35">
       <c r="B30" s="13" t="s">
         <v>5</v>
       </c>
@@ -2986,7 +3005,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B31" s="13" t="s">
         <v>188</v>
       </c>
@@ -3011,7 +3030,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="11" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B32" s="13" t="s">
         <v>189</v>
       </c>
@@ -3040,7 +3059,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="11" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" s="11" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B33" s="13" t="s">
         <v>192</v>
       </c>
@@ -3069,7 +3088,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="13" t="s">
         <v>195</v>
       </c>
@@ -3098,7 +3117,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13" t="s">
         <v>198</v>
@@ -3126,7 +3145,7 @@
       <c r="Q35" s="13"/>
       <c r="R35" s="14"/>
     </row>
-    <row r="36" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="13" t="s">
         <v>199</v>
@@ -3154,7 +3173,7 @@
       <c r="Q36" s="13"/>
       <c r="R36" s="14"/>
     </row>
-    <row r="37" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13" t="s">
         <v>200</v>
@@ -3182,7 +3201,7 @@
       <c r="Q37" s="13"/>
       <c r="R37" s="14"/>
     </row>
-    <row r="38" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="13" t="s">
         <v>201</v>
@@ -3210,7 +3229,7 @@
       <c r="Q38" s="13"/>
       <c r="R38" s="14"/>
     </row>
-    <row r="39" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
         <v>202</v>
@@ -3238,7 +3257,7 @@
       <c r="Q39" s="13"/>
       <c r="R39" s="14"/>
     </row>
-    <row r="40" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
         <v>203</v>
@@ -3266,7 +3285,7 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="14"/>
     </row>
-    <row r="41" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13" t="s">
         <v>204</v>
@@ -3294,7 +3313,7 @@
       <c r="Q41" s="13"/>
       <c r="R41" s="14"/>
     </row>
-    <row r="42" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
         <v>205</v>
@@ -3322,7 +3341,7 @@
       <c r="Q42" s="13"/>
       <c r="R42" s="14"/>
     </row>
-    <row r="43" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="13" t="s">
         <v>206</v>
@@ -3350,7 +3369,7 @@
       <c r="Q43" s="13"/>
       <c r="R43" s="14"/>
     </row>
-    <row r="44" spans="1:18" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>147</v>
       </c>
@@ -3382,7 +3401,7 @@
       <c r="Q44" s="13"/>
       <c r="R44" s="14"/>
     </row>
-    <row r="45" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12"/>
       <c r="B45" s="13" t="s">
         <v>207</v>
@@ -3410,7 +3429,7 @@
       <c r="Q45" s="12"/>
       <c r="R45" s="12"/>
     </row>
-    <row r="46" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="13" t="s">
         <v>208</v>
@@ -3438,7 +3457,7 @@
       <c r="Q46" s="12"/>
       <c r="R46" s="14"/>
     </row>
-    <row r="47" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="13" t="s">
         <v>209</v>
@@ -3466,7 +3485,7 @@
       <c r="Q47" s="12"/>
       <c r="R47" s="12"/>
     </row>
-    <row r="48" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B48" s="13" t="s">
         <v>210</v>
       </c>
@@ -3492,7 +3511,7 @@
       </c>
       <c r="Q48" s="13"/>
     </row>
-    <row r="49" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="13" t="s">
         <v>211</v>
       </c>
@@ -3518,7 +3537,7 @@
       </c>
       <c r="Q49" s="13"/>
     </row>
-    <row r="50" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="13" t="s">
         <v>212</v>
       </c>
@@ -3543,7 +3562,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="13" t="s">
         <v>213</v>
       </c>
@@ -3568,7 +3587,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
       <c r="B52" s="13" t="s">
         <v>139</v>
@@ -3596,7 +3615,7 @@
       <c r="Q52" s="13"/>
       <c r="R52" s="14"/>
     </row>
-    <row r="53" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="12"/>
       <c r="B53" s="13" t="s">
         <v>214</v>
@@ -3623,7 +3642,7 @@
       </c>
       <c r="R53" s="12"/>
     </row>
-    <row r="54" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="13" t="s">
         <v>215</v>
       </c>
@@ -3648,7 +3667,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B55" s="13" t="s">
         <v>216</v>
       </c>
@@ -3674,7 +3693,7 @@
       </c>
       <c r="Q55" s="12"/>
     </row>
-    <row r="56" spans="1:18" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:18" s="11" customFormat="1" ht="54" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>508</v>
       </c>
@@ -3705,7 +3724,7 @@
       <c r="P56" s="13"/>
       <c r="Q56" s="12"/>
     </row>
-    <row r="57" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B57" s="13" t="s">
         <v>511</v>
       </c>
@@ -3737,7 +3756,7 @@
       </c>
       <c r="Q57" s="13"/>
     </row>
-    <row r="58" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B58" s="13" t="s">
         <v>217</v>
       </c>
@@ -3763,7 +3782,7 @@
       </c>
       <c r="Q58" s="13"/>
     </row>
-    <row r="59" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13"/>
       <c r="B59" s="13" t="s">
         <v>218</v>
@@ -3790,7 +3809,7 @@
       </c>
       <c r="R59" s="14"/>
     </row>
-    <row r="60" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12"/>
       <c r="B60" s="13" t="s">
         <v>219</v>
@@ -3817,7 +3836,7 @@
       </c>
       <c r="R60" s="12"/>
     </row>
-    <row r="61" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="12"/>
       <c r="B61" s="13" t="s">
         <v>220</v>
@@ -3844,7 +3863,7 @@
       </c>
       <c r="R61" s="12"/>
     </row>
-    <row r="62" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B62" s="13" t="s">
         <v>221</v>
       </c>
@@ -3869,7 +3888,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B63" s="13" t="s">
         <v>222</v>
       </c>
@@ -3894,33 +3913,37 @@
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B64" s="13" t="s">
+    <row r="64" spans="1:18" s="19" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13">
-        <v>1</v>
-      </c>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q64" s="12"/>
-    </row>
-    <row r="65" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C64" s="21" t="s">
+        <v>529</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
+      <c r="N64" s="21">
+        <v>1</v>
+      </c>
+      <c r="O64" s="21"/>
+      <c r="P64" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q64" s="23"/>
+    </row>
+    <row r="65" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B65" s="13" t="s">
         <v>224</v>
       </c>
@@ -3945,7 +3968,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B66" s="13" t="s">
         <v>225</v>
       </c>
@@ -3971,7 +3994,7 @@
       </c>
       <c r="Q66" s="13"/>
     </row>
-    <row r="67" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="12"/>
       <c r="B67" s="13" t="s">
         <v>226</v>
@@ -3999,7 +4022,7 @@
       <c r="Q67" s="13"/>
       <c r="R67" s="12"/>
     </row>
-    <row r="68" spans="1:19" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11"/>
       <c r="B68" s="13" t="s">
         <v>227</v>
@@ -4028,7 +4051,7 @@
       <c r="R68" s="11"/>
       <c r="S68" s="11"/>
     </row>
-    <row r="69" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="13" t="s">
         <v>228</v>
@@ -4056,7 +4079,7 @@
       <c r="Q69" s="13"/>
       <c r="R69" s="14"/>
     </row>
-    <row r="70" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
       <c r="B70" s="13" t="s">
         <v>229</v>
@@ -4084,7 +4107,7 @@
       <c r="Q70" s="13"/>
       <c r="R70" s="14"/>
     </row>
-    <row r="71" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
       <c r="B71" s="13" t="s">
         <v>230</v>
@@ -4112,7 +4135,7 @@
       <c r="Q71" s="13"/>
       <c r="R71" s="14"/>
     </row>
-    <row r="72" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
       <c r="B72" s="13" t="s">
         <v>518</v>
@@ -4146,7 +4169,7 @@
       <c r="Q72" s="13"/>
       <c r="R72" s="14"/>
     </row>
-    <row r="73" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
       <c r="B73" s="13" t="s">
         <v>513</v>
@@ -4176,7 +4199,7 @@
       <c r="Q73" s="13"/>
       <c r="R73" s="14"/>
     </row>
-    <row r="74" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="13"/>
       <c r="B74" s="13" t="s">
         <v>514</v>
@@ -4206,7 +4229,7 @@
       <c r="Q74" s="13"/>
       <c r="R74" s="14"/>
     </row>
-    <row r="75" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="13" t="s">
         <v>231</v>
@@ -4233,7 +4256,7 @@
       </c>
       <c r="R75" s="14"/>
     </row>
-    <row r="76" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
       <c r="B76" s="13" t="s">
         <v>232</v>
@@ -4260,7 +4283,7 @@
       </c>
       <c r="R76" s="14"/>
     </row>
-    <row r="77" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B77" s="13" t="s">
         <v>233</v>
       </c>
@@ -4285,7 +4308,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B78" s="13" t="s">
         <v>234</v>
       </c>
@@ -4311,7 +4334,7 @@
       </c>
       <c r="Q78" s="13"/>
     </row>
-    <row r="79" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B79" s="13" t="s">
         <v>235</v>
       </c>
@@ -4337,7 +4360,7 @@
       </c>
       <c r="Q79" s="13"/>
     </row>
-    <row r="80" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="13"/>
       <c r="B80" s="13" t="s">
         <v>236</v>
@@ -4364,7 +4387,7 @@
       </c>
       <c r="R80" s="14"/>
     </row>
-    <row r="81" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B81" s="13" t="s">
         <v>237</v>
       </c>
@@ -4391,7 +4414,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
       <c r="B82" s="13" t="s">
         <v>239</v>
@@ -4419,7 +4442,7 @@
       <c r="Q82" s="13"/>
       <c r="R82" s="14"/>
     </row>
-    <row r="83" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
       <c r="B83" s="13" t="s">
         <v>240</v>
@@ -4447,7 +4470,7 @@
       <c r="Q83" s="13"/>
       <c r="R83" s="14"/>
     </row>
-    <row r="84" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B84" s="13" t="s">
         <v>241</v>
       </c>
@@ -4475,7 +4498,7 @@
       </c>
       <c r="Q84" s="13"/>
     </row>
-    <row r="85" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B85" s="13" t="s">
         <v>243</v>
       </c>
@@ -4506,7 +4529,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
       <c r="B86" s="11" t="s">
         <v>425</v>
@@ -4533,7 +4556,7 @@
       </c>
       <c r="R86" s="14"/>
     </row>
-    <row r="87" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B87" s="13" t="s">
         <v>247</v>
       </c>
@@ -4558,7 +4581,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B88" s="13" t="s">
         <v>248</v>
       </c>
@@ -4585,7 +4608,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
       <c r="B89" s="13" t="s">
         <v>250</v>
@@ -4614,7 +4637,7 @@
       </c>
       <c r="R89" s="14"/>
     </row>
-    <row r="90" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B90" s="13" t="s">
         <v>252</v>
       </c>
@@ -4639,7 +4662,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B91" s="13" t="s">
         <v>253</v>
       </c>
@@ -4665,7 +4688,7 @@
       </c>
       <c r="Q91" s="13"/>
     </row>
-    <row r="92" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B92" s="13" t="s">
         <v>254</v>
       </c>
@@ -4691,7 +4714,7 @@
       </c>
       <c r="Q92" s="13"/>
     </row>
-    <row r="93" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B93" s="13" t="s">
         <v>255</v>
       </c>
@@ -4717,7 +4740,7 @@
       </c>
       <c r="Q93" s="13"/>
     </row>
-    <row r="94" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="13"/>
       <c r="B94" s="13" t="s">
         <v>256</v>
@@ -4746,7 +4769,7 @@
       </c>
       <c r="R94" s="14"/>
     </row>
-    <row r="95" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B95" s="13" t="s">
         <v>258</v>
       </c>
@@ -4771,7 +4794,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="96" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B96" s="13" t="s">
         <v>259</v>
       </c>
@@ -4796,7 +4819,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B97" s="13" t="s">
         <v>260</v>
       </c>
@@ -4821,7 +4844,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B98" s="13" t="s">
         <v>261</v>
       </c>
@@ -4846,7 +4869,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B99" s="13" t="s">
         <v>262</v>
       </c>
@@ -4871,7 +4894,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="13"/>
       <c r="B100" s="13" t="s">
         <v>263</v>
@@ -4899,7 +4922,7 @@
       <c r="Q100" s="13"/>
       <c r="R100" s="14"/>
     </row>
-    <row r="101" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B101" s="13" t="s">
         <v>264</v>
       </c>
@@ -4925,7 +4948,7 @@
       </c>
       <c r="Q101" s="13"/>
     </row>
-    <row r="102" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="13"/>
       <c r="B102" s="13" t="s">
         <v>265</v>
@@ -4952,7 +4975,7 @@
       </c>
       <c r="R102" s="14"/>
     </row>
-    <row r="103" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="13" t="s">
         <v>266</v>
@@ -4979,7 +5002,7 @@
       </c>
       <c r="R103" s="14"/>
     </row>
-    <row r="104" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="13"/>
       <c r="B104" s="13" t="s">
         <v>267</v>
@@ -5006,7 +5029,7 @@
       </c>
       <c r="R104" s="14"/>
     </row>
-    <row r="105" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B105" s="13" t="s">
         <v>268</v>
       </c>
@@ -5031,7 +5054,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="106" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B106" s="11" t="s">
         <v>466</v>
       </c>
@@ -5056,7 +5079,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="107" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B107" s="13" t="s">
         <v>271</v>
       </c>
@@ -5081,7 +5104,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B108" s="11" t="s">
         <v>467</v>
       </c>
@@ -5106,7 +5129,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="109" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B109" s="11" t="s">
         <v>468</v>
       </c>
@@ -5131,7 +5154,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="110" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="12"/>
       <c r="B110" s="11" t="s">
         <v>295</v>
@@ -5155,7 +5178,7 @@
       <c r="R110" s="12"/>
       <c r="S110" s="12"/>
     </row>
-    <row r="111" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B111" s="11" t="s">
         <v>496</v>
       </c>
@@ -5181,7 +5204,7 @@
       <c r="R111" s="12"/>
       <c r="S111" s="12"/>
     </row>
-    <row r="112" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="12"/>
       <c r="B112" s="11" t="s">
         <v>341</v>
@@ -5205,7 +5228,7 @@
       <c r="R112" s="12"/>
       <c r="S112" s="12"/>
     </row>
-    <row r="113" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="12"/>
       <c r="B113" s="11" t="s">
         <v>299</v>
@@ -5223,7 +5246,7 @@
       <c r="R113" s="12"/>
       <c r="S113" s="12"/>
     </row>
-    <row r="114" spans="1:19" s="11" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:19" s="11" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B114" s="12" t="s">
         <v>79</v>
       </c>
@@ -5255,7 +5278,7 @@
       <c r="P114" s="12"/>
       <c r="S114" s="13"/>
     </row>
-    <row r="115" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B115" s="11" t="s">
         <v>301</v>
       </c>
@@ -5267,7 +5290,7 @@
       </c>
       <c r="S115" s="13"/>
     </row>
-    <row r="116" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B116" s="12" t="s">
         <v>75</v>
       </c>
@@ -5297,7 +5320,7 @@
       <c r="P116" s="12"/>
       <c r="S116" s="13"/>
     </row>
-    <row r="117" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A117" s="13"/>
       <c r="B117" s="12" t="s">
         <v>91</v>
@@ -5330,7 +5353,7 @@
       <c r="R117" s="14"/>
       <c r="S117" s="13"/>
     </row>
-    <row r="118" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="12"/>
       <c r="B118" s="11" t="s">
         <v>302</v>
@@ -5345,7 +5368,7 @@
       <c r="R118" s="12"/>
       <c r="S118" s="13"/>
     </row>
-    <row r="119" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A119" s="13"/>
       <c r="B119" s="12" t="s">
         <v>80</v>
@@ -5378,7 +5401,7 @@
       <c r="R119" s="14"/>
       <c r="S119" s="13"/>
     </row>
-    <row r="120" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B120" s="11" t="s">
         <v>303</v>
       </c>
@@ -5390,7 +5413,7 @@
       </c>
       <c r="S120" s="13"/>
     </row>
-    <row r="121" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="12"/>
       <c r="B121" s="11" t="s">
         <v>304</v>
@@ -5405,7 +5428,7 @@
       <c r="R121" s="12"/>
       <c r="S121" s="13"/>
     </row>
-    <row r="122" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B122" s="11" t="s">
         <v>305</v>
       </c>
@@ -5417,7 +5440,7 @@
       </c>
       <c r="S122" s="13"/>
     </row>
-    <row r="123" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" s="12"/>
       <c r="B123" s="11" t="s">
         <v>306</v>
@@ -5432,7 +5455,7 @@
       <c r="R123" s="12"/>
       <c r="S123" s="13"/>
     </row>
-    <row r="124" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B124" s="11" t="s">
         <v>307</v>
       </c>
@@ -5444,7 +5467,7 @@
       </c>
       <c r="S124" s="13"/>
     </row>
-    <row r="125" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="12"/>
       <c r="B125" s="11" t="s">
         <v>308</v>
@@ -5459,7 +5482,7 @@
       <c r="R125" s="12"/>
       <c r="S125" s="13"/>
     </row>
-    <row r="126" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B126" s="11" t="s">
         <v>309</v>
       </c>
@@ -5471,7 +5494,7 @@
       </c>
       <c r="S126" s="13"/>
     </row>
-    <row r="127" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B127" s="11" t="s">
         <v>310</v>
       </c>
@@ -5483,7 +5506,7 @@
       </c>
       <c r="S127" s="13"/>
     </row>
-    <row r="128" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B128" s="11" t="s">
         <v>311</v>
       </c>
@@ -5495,7 +5518,7 @@
       </c>
       <c r="S128" s="13"/>
     </row>
-    <row r="129" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B129" s="11" t="s">
         <v>312</v>
       </c>
@@ -5507,7 +5530,7 @@
       </c>
       <c r="S129" s="13"/>
     </row>
-    <row r="130" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B130" s="11" t="s">
         <v>313</v>
       </c>
@@ -5519,7 +5542,7 @@
       </c>
       <c r="S130" s="13"/>
     </row>
-    <row r="131" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="13"/>
       <c r="B131" s="11" t="s">
         <v>314</v>
@@ -5534,7 +5557,7 @@
       <c r="R131" s="14"/>
       <c r="S131" s="13"/>
     </row>
-    <row r="132" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B132" s="11" t="s">
         <v>315</v>
       </c>
@@ -5546,7 +5569,7 @@
       </c>
       <c r="S132" s="13"/>
     </row>
-    <row r="133" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B133" s="11" t="s">
         <v>316</v>
       </c>
@@ -5558,7 +5581,7 @@
       </c>
       <c r="S133" s="13"/>
     </row>
-    <row r="134" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B134" s="11" t="s">
         <v>317</v>
       </c>
@@ -5570,7 +5593,7 @@
       </c>
       <c r="S134" s="13"/>
     </row>
-    <row r="135" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B135" s="11" t="s">
         <v>318</v>
       </c>
@@ -5582,7 +5605,7 @@
       </c>
       <c r="S135" s="13"/>
     </row>
-    <row r="136" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B136" s="11" t="s">
         <v>319</v>
       </c>
@@ -5594,7 +5617,7 @@
       </c>
       <c r="S136" s="13"/>
     </row>
-    <row r="137" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B137" s="11" t="s">
         <v>320</v>
       </c>
@@ -5606,7 +5629,7 @@
       </c>
       <c r="S137" s="13"/>
     </row>
-    <row r="138" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="13"/>
       <c r="B138" s="11" t="s">
         <v>321</v>
@@ -5621,7 +5644,7 @@
       <c r="R138" s="14"/>
       <c r="S138" s="13"/>
     </row>
-    <row r="139" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B139" s="11" t="s">
         <v>322</v>
       </c>
@@ -5633,7 +5656,7 @@
       </c>
       <c r="S139" s="13"/>
     </row>
-    <row r="140" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B140" s="11" t="s">
         <v>323</v>
       </c>
@@ -5645,7 +5668,7 @@
       </c>
       <c r="S140" s="13"/>
     </row>
-    <row r="141" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B141" s="11" t="s">
         <v>324</v>
       </c>
@@ -5657,7 +5680,7 @@
       </c>
       <c r="S141" s="13"/>
     </row>
-    <row r="142" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B142" s="11" t="s">
         <v>325</v>
       </c>
@@ -5669,7 +5692,7 @@
       </c>
       <c r="S142" s="13"/>
     </row>
-    <row r="143" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B143" s="11" t="s">
         <v>326</v>
       </c>
@@ -5681,7 +5704,7 @@
       </c>
       <c r="S143" s="13"/>
     </row>
-    <row r="144" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B144" s="11" t="s">
         <v>327</v>
       </c>
@@ -5693,7 +5716,7 @@
       </c>
       <c r="S144" s="13"/>
     </row>
-    <row r="145" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B145" s="11" t="s">
         <v>328</v>
       </c>
@@ -5705,7 +5728,7 @@
       </c>
       <c r="S145" s="13"/>
     </row>
-    <row r="146" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B146" s="11" t="s">
         <v>329</v>
       </c>
@@ -5717,7 +5740,7 @@
       </c>
       <c r="S146" s="13"/>
     </row>
-    <row r="147" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B147" s="11" t="s">
         <v>330</v>
       </c>
@@ -5729,7 +5752,7 @@
       </c>
       <c r="S147" s="13"/>
     </row>
-    <row r="148" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B148" s="12" t="s">
         <v>66</v>
       </c>
@@ -5757,7 +5780,7 @@
       <c r="P148" s="12"/>
       <c r="S148" s="13"/>
     </row>
-    <row r="149" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="13"/>
       <c r="B149" s="11" t="s">
         <v>331</v>
@@ -5772,7 +5795,7 @@
       <c r="R149" s="14"/>
       <c r="S149" s="13"/>
     </row>
-    <row r="150" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B150" s="11" t="s">
         <v>332</v>
       </c>
@@ -5784,7 +5807,7 @@
       </c>
       <c r="S150" s="13"/>
     </row>
-    <row r="151" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B151" s="12" t="s">
         <v>130</v>
       </c>
@@ -5812,7 +5835,7 @@
       <c r="P151" s="12"/>
       <c r="S151" s="13"/>
     </row>
-    <row r="152" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B152" s="11" t="s">
         <v>333</v>
       </c>
@@ -5824,7 +5847,7 @@
       </c>
       <c r="S152" s="13"/>
     </row>
-    <row r="153" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B153" s="16" t="s">
         <v>275</v>
       </c>
@@ -5851,7 +5874,7 @@
       </c>
       <c r="S153" s="13"/>
     </row>
-    <row r="154" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A154" s="12"/>
       <c r="B154" s="11" t="s">
         <v>334</v>
@@ -5869,7 +5892,7 @@
       <c r="R154" s="12"/>
       <c r="S154" s="13"/>
     </row>
-    <row r="155" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B155" s="11" t="s">
         <v>336</v>
       </c>
@@ -5881,7 +5904,7 @@
       </c>
       <c r="S155" s="13"/>
     </row>
-    <row r="156" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B156" s="16" t="s">
         <v>474</v>
       </c>
@@ -5908,7 +5931,7 @@
       </c>
       <c r="S156" s="13"/>
     </row>
-    <row r="157" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="12"/>
       <c r="B157" s="11" t="s">
         <v>337</v>
@@ -5923,7 +5946,7 @@
       <c r="R157" s="12"/>
       <c r="S157" s="13"/>
     </row>
-    <row r="158" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B158" s="11" t="s">
         <v>338</v>
       </c>
@@ -5935,7 +5958,7 @@
       </c>
       <c r="S158" s="13"/>
     </row>
-    <row r="159" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B159" s="11" t="s">
         <v>339</v>
       </c>
@@ -5956,7 +5979,7 @@
       </c>
       <c r="S159" s="13"/>
     </row>
-    <row r="160" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B160" s="11" t="s">
         <v>342</v>
       </c>
@@ -5968,7 +5991,7 @@
       </c>
       <c r="S160" s="13"/>
     </row>
-    <row r="161" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B161" s="11" t="s">
         <v>343</v>
       </c>
@@ -5980,7 +6003,7 @@
       </c>
       <c r="S161" s="13"/>
     </row>
-    <row r="162" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B162" s="11" t="s">
         <v>344</v>
       </c>
@@ -5992,7 +6015,7 @@
       </c>
       <c r="S162" s="13"/>
     </row>
-    <row r="163" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B163" s="11" t="s">
         <v>345</v>
       </c>
@@ -6004,7 +6027,7 @@
       </c>
       <c r="S163" s="13"/>
     </row>
-    <row r="164" spans="1:19" s="11" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:19" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B164" s="12" t="s">
         <v>62</v>
       </c>
@@ -6034,7 +6057,7 @@
       <c r="P164" s="12"/>
       <c r="S164" s="13"/>
     </row>
-    <row r="165" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B165" s="11" t="s">
         <v>346</v>
       </c>
@@ -6046,7 +6069,7 @@
       </c>
       <c r="S165" s="13"/>
     </row>
-    <row r="166" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B166" s="11" t="s">
         <v>347</v>
       </c>
@@ -6058,7 +6081,7 @@
       </c>
       <c r="S166" s="13"/>
     </row>
-    <row r="167" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B167" s="11" t="s">
         <v>348</v>
       </c>
@@ -6070,7 +6093,7 @@
       </c>
       <c r="S167" s="13"/>
     </row>
-    <row r="168" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B168" s="11" t="s">
         <v>349</v>
       </c>
@@ -6082,7 +6105,7 @@
       </c>
       <c r="S168" s="13"/>
     </row>
-    <row r="169" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A169" s="12"/>
       <c r="B169" s="11" t="s">
         <v>350</v>
@@ -6097,7 +6120,7 @@
       <c r="R169" s="12"/>
       <c r="S169" s="13"/>
     </row>
-    <row r="170" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B170" s="11" t="s">
         <v>351</v>
       </c>
@@ -6109,7 +6132,7 @@
       </c>
       <c r="S170" s="13"/>
     </row>
-    <row r="171" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B171" s="11" t="s">
         <v>352</v>
       </c>
@@ -6121,7 +6144,7 @@
       </c>
       <c r="S171" s="13"/>
     </row>
-    <row r="172" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B172" s="11" t="s">
         <v>353</v>
       </c>
@@ -6133,7 +6156,7 @@
       </c>
       <c r="S172" s="13"/>
     </row>
-    <row r="173" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:19" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B173" s="11" t="s">
         <v>354</v>
       </c>
@@ -6154,7 +6177,7 @@
       </c>
       <c r="S173" s="13"/>
     </row>
-    <row r="174" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B174" s="13" t="s">
         <v>273</v>
       </c>
@@ -6167,7 +6190,7 @@
       <c r="Q174" s="13"/>
       <c r="S174" s="13"/>
     </row>
-    <row r="175" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A175" s="13"/>
       <c r="B175" s="11" t="s">
         <v>356</v>
@@ -6182,7 +6205,7 @@
       <c r="R175" s="14"/>
       <c r="S175" s="13"/>
     </row>
-    <row r="176" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B176" s="12" t="s">
         <v>78</v>
       </c>
@@ -6210,7 +6233,7 @@
       <c r="P176" s="12"/>
       <c r="S176" s="13"/>
     </row>
-    <row r="177" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B177" s="11" t="s">
         <v>357</v>
       </c>
@@ -6222,7 +6245,7 @@
       </c>
       <c r="S177" s="13"/>
     </row>
-    <row r="178" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B178" s="11" t="s">
         <v>358</v>
       </c>
@@ -6233,7 +6256,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="179" spans="1:19" s="11" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:19" s="11" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B179" s="12" t="s">
         <v>131</v>
       </c>
@@ -6262,7 +6285,7 @@
       <c r="O179" s="12"/>
       <c r="P179" s="12"/>
     </row>
-    <row r="180" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B180" s="11" t="s">
         <v>359</v>
       </c>
@@ -6273,7 +6296,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="181" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B181" s="11" t="s">
         <v>360</v>
       </c>
@@ -6284,7 +6307,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="182" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A182" s="12"/>
       <c r="B182" s="11" t="s">
         <v>361</v>
@@ -6298,7 +6321,7 @@
       <c r="Q182" s="12"/>
       <c r="R182" s="12"/>
     </row>
-    <row r="183" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B183" s="16" t="s">
         <v>279</v>
       </c>
@@ -6324,7 +6347,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="184" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B184" s="11" t="s">
         <v>362</v>
       </c>
@@ -6335,7 +6358,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="185" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B185" s="16" t="s">
         <v>281</v>
       </c>
@@ -6361,7 +6384,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="186" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A186" s="13"/>
       <c r="B186" s="11" t="s">
         <v>363</v>
@@ -6375,7 +6398,7 @@
       <c r="Q186" s="13"/>
       <c r="R186" s="14"/>
     </row>
-    <row r="187" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A187" s="13"/>
       <c r="B187" s="11" t="s">
         <v>364</v>
@@ -6389,7 +6412,7 @@
       <c r="Q187" s="13"/>
       <c r="R187" s="14"/>
     </row>
-    <row r="188" spans="1:19" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:19" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B188" s="16" t="s">
         <v>473</v>
       </c>
@@ -6415,7 +6438,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="189" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B189" s="16" t="s">
         <v>283</v>
       </c>
@@ -6441,7 +6464,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="190" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="13"/>
       <c r="B190" s="11" t="s">
         <v>365</v>
@@ -6455,7 +6478,7 @@
       <c r="Q190" s="13"/>
       <c r="R190" s="14"/>
     </row>
-    <row r="191" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B191" s="11" t="s">
         <v>366</v>
       </c>
@@ -6466,7 +6489,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="192" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B192" s="11" t="s">
         <v>367</v>
       </c>
@@ -6477,7 +6500,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="193" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="13"/>
       <c r="B193" s="16" t="s">
         <v>479</v>
@@ -6506,7 +6529,7 @@
       <c r="Q193" s="13"/>
       <c r="R193" s="14"/>
     </row>
-    <row r="194" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B194" s="16" t="s">
         <v>493</v>
       </c>
@@ -6532,7 +6555,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="195" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B195" s="11" t="s">
         <v>368</v>
       </c>
@@ -6543,7 +6566,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="196" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A196" s="13"/>
       <c r="B196" s="11" t="s">
         <v>369</v>
@@ -6557,7 +6580,7 @@
       <c r="Q196" s="13"/>
       <c r="R196" s="14"/>
     </row>
-    <row r="197" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A197" s="13"/>
       <c r="B197" s="11" t="s">
         <v>370</v>
@@ -6574,7 +6597,7 @@
       <c r="Q197" s="13"/>
       <c r="R197" s="14"/>
     </row>
-    <row r="198" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="13"/>
       <c r="B198" s="11" t="s">
         <v>372</v>
@@ -6591,7 +6614,7 @@
       <c r="Q198" s="13"/>
       <c r="R198" s="14"/>
     </row>
-    <row r="199" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A199" s="13"/>
       <c r="B199" s="16" t="s">
         <v>285</v>
@@ -6620,7 +6643,7 @@
       <c r="Q199" s="13"/>
       <c r="R199" s="14"/>
     </row>
-    <row r="200" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B200" s="11" t="s">
         <v>374</v>
       </c>
@@ -6631,7 +6654,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="201" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B201" s="11" t="s">
         <v>375</v>
       </c>
@@ -6642,7 +6665,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="202" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A202" s="13"/>
       <c r="B202" s="11" t="s">
         <v>376</v>
@@ -6656,7 +6679,7 @@
       <c r="Q202" s="13"/>
       <c r="R202" s="14"/>
     </row>
-    <row r="203" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A203" s="13"/>
       <c r="B203" s="11" t="s">
         <v>377</v>
@@ -6670,7 +6693,7 @@
       <c r="Q203" s="13"/>
       <c r="R203" s="14"/>
     </row>
-    <row r="204" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A204" s="12"/>
       <c r="B204" s="11" t="s">
         <v>189</v>
@@ -6687,7 +6710,7 @@
       <c r="Q204" s="12"/>
       <c r="R204" s="12"/>
     </row>
-    <row r="205" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A205" s="13"/>
       <c r="B205" s="12" t="s">
         <v>60</v>
@@ -6717,7 +6740,7 @@
       <c r="Q205" s="13"/>
       <c r="R205" s="14"/>
     </row>
-    <row r="206" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A206" s="13"/>
       <c r="B206" s="12" t="s">
         <v>67</v>
@@ -6747,7 +6770,7 @@
       <c r="Q206" s="13"/>
       <c r="R206" s="14"/>
     </row>
-    <row r="207" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="13"/>
       <c r="B207" s="11" t="s">
         <v>378</v>
@@ -6761,7 +6784,7 @@
       <c r="Q207" s="13"/>
       <c r="R207" s="14"/>
     </row>
-    <row r="208" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A208" s="13"/>
       <c r="B208" s="12" t="s">
         <v>143</v>
@@ -6791,7 +6814,7 @@
       <c r="Q208" s="13"/>
       <c r="R208" s="14"/>
     </row>
-    <row r="209" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A209" s="13"/>
       <c r="B209" s="11" t="s">
         <v>379</v>
@@ -6804,7 +6827,7 @@
       </c>
       <c r="R209" s="14"/>
     </row>
-    <row r="210" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A210" s="12"/>
       <c r="B210" s="11" t="s">
         <v>380</v>
@@ -6817,7 +6840,7 @@
       </c>
       <c r="R210" s="12"/>
     </row>
-    <row r="211" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A211" s="12"/>
       <c r="B211" s="11" t="s">
         <v>381</v>
@@ -6831,7 +6854,7 @@
       <c r="Q211" s="13"/>
       <c r="R211" s="12"/>
     </row>
-    <row r="212" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A212" s="13"/>
       <c r="B212" s="11" t="s">
         <v>382</v>
@@ -6844,7 +6867,7 @@
       </c>
       <c r="R212" s="14"/>
     </row>
-    <row r="213" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" s="13"/>
       <c r="B213" s="11" t="s">
         <v>383</v>
@@ -6858,7 +6881,7 @@
       <c r="Q213" s="13"/>
       <c r="R213" s="14"/>
     </row>
-    <row r="214" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B214" s="11" t="s">
         <v>384</v>
       </c>
@@ -6870,7 +6893,7 @@
       </c>
       <c r="Q214" s="13"/>
     </row>
-    <row r="215" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" s="13"/>
       <c r="B215" s="11" t="s">
         <v>385</v>
@@ -6883,7 +6906,7 @@
       </c>
       <c r="R215" s="14"/>
     </row>
-    <row r="216" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" s="13"/>
       <c r="B216" s="11" t="s">
         <v>386</v>
@@ -6896,7 +6919,7 @@
       </c>
       <c r="R216" s="14"/>
     </row>
-    <row r="217" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="13"/>
       <c r="B217" s="11" t="s">
         <v>387</v>
@@ -6909,7 +6932,7 @@
       </c>
       <c r="R217" s="14"/>
     </row>
-    <row r="218" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B218" s="11" t="s">
         <v>388</v>
       </c>
@@ -6921,7 +6944,7 @@
       </c>
       <c r="Q218" s="13"/>
     </row>
-    <row r="219" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B219" s="11" t="s">
         <v>389</v>
       </c>
@@ -6932,7 +6955,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="220" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="13"/>
       <c r="B220" s="12" t="s">
         <v>77</v>
@@ -6955,7 +6978,7 @@
       <c r="P220" s="12"/>
       <c r="R220" s="14"/>
     </row>
-    <row r="221" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B221" s="16" t="s">
         <v>287</v>
       </c>
@@ -6981,7 +7004,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="222" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B222" s="11" t="s">
         <v>390</v>
       </c>
@@ -6992,7 +7015,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="223" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B223" s="11" t="s">
         <v>391</v>
       </c>
@@ -7003,7 +7026,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="224" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B224" s="11" t="s">
         <v>392</v>
       </c>
@@ -7015,7 +7038,7 @@
       </c>
       <c r="Q224" s="13"/>
     </row>
-    <row r="225" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B225" s="11" t="s">
         <v>393</v>
       </c>
@@ -7027,7 +7050,7 @@
       </c>
       <c r="Q225" s="12"/>
     </row>
-    <row r="226" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B226" s="12" t="s">
         <v>138</v>
       </c>
@@ -7054,7 +7077,7 @@
       <c r="O226" s="12"/>
       <c r="P226" s="12"/>
     </row>
-    <row r="227" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A227" s="13"/>
       <c r="B227" s="11" t="s">
         <v>394</v>
@@ -7070,7 +7093,7 @@
       </c>
       <c r="R227" s="14"/>
     </row>
-    <row r="228" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B228" s="11" t="s">
         <v>396</v>
       </c>
@@ -7081,7 +7104,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="229" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A229" s="12"/>
       <c r="B229" s="11" t="s">
         <v>397</v>
@@ -7095,7 +7118,7 @@
       <c r="Q229" s="13"/>
       <c r="R229" s="12"/>
     </row>
-    <row r="230" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A230" s="13"/>
       <c r="B230" s="11" t="s">
         <v>398</v>
@@ -7108,7 +7131,7 @@
       </c>
       <c r="R230" s="14"/>
     </row>
-    <row r="231" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A231" s="13"/>
       <c r="B231" s="11" t="s">
         <v>399</v>
@@ -7122,7 +7145,7 @@
       <c r="Q231" s="13"/>
       <c r="R231" s="14"/>
     </row>
-    <row r="232" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B232" s="11" t="s">
         <v>400</v>
       </c>
@@ -7134,7 +7157,7 @@
       </c>
       <c r="Q232" s="13"/>
     </row>
-    <row r="233" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B233" s="11" t="s">
         <v>401</v>
       </c>
@@ -7146,7 +7169,7 @@
       </c>
       <c r="Q233" s="13"/>
     </row>
-    <row r="234" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A234" s="13"/>
       <c r="B234" s="11" t="s">
         <v>402</v>
@@ -7159,7 +7182,7 @@
       </c>
       <c r="R234" s="14"/>
     </row>
-    <row r="235" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A235" s="13"/>
       <c r="B235" s="12" t="s">
         <v>69</v>
@@ -7192,7 +7215,7 @@
       <c r="P235" s="12"/>
       <c r="R235" s="14"/>
     </row>
-    <row r="236" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B236" s="12" t="s">
         <v>63</v>
       </c>
@@ -7213,7 +7236,7 @@
       <c r="O236" s="12"/>
       <c r="P236" s="12"/>
     </row>
-    <row r="237" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A237" s="13"/>
       <c r="B237" s="12" t="s">
         <v>64</v>
@@ -7236,7 +7259,7 @@
       <c r="P237" s="12"/>
       <c r="R237" s="14"/>
     </row>
-    <row r="238" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B238" s="12" t="s">
         <v>59</v>
       </c>
@@ -7263,7 +7286,7 @@
       <c r="O238" s="12"/>
       <c r="P238" s="12"/>
     </row>
-    <row r="239" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B239" s="11" t="s">
         <v>403</v>
       </c>
@@ -7274,7 +7297,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="240" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B240" s="11" t="s">
         <v>404</v>
       </c>
@@ -7288,7 +7311,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="241" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B241" s="11" t="s">
         <v>406</v>
       </c>
@@ -7300,7 +7323,7 @@
       </c>
       <c r="Q241" s="12"/>
     </row>
-    <row r="242" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B242" s="11" t="s">
         <v>407</v>
       </c>
@@ -7312,7 +7335,7 @@
       </c>
       <c r="Q242" s="12"/>
     </row>
-    <row r="243" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B243" s="11" t="s">
         <v>408</v>
       </c>
@@ -7324,7 +7347,7 @@
       </c>
       <c r="Q243" s="12"/>
     </row>
-    <row r="244" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="12"/>
       <c r="B244" s="12" t="s">
         <v>65</v>
@@ -7348,7 +7371,7 @@
       <c r="Q244" s="12"/>
       <c r="R244" s="12"/>
     </row>
-    <row r="245" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A245" s="12"/>
       <c r="B245" s="16" t="s">
         <v>289</v>
@@ -7376,7 +7399,7 @@
       </c>
       <c r="R245" s="12"/>
     </row>
-    <row r="246" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A246" s="13"/>
       <c r="B246" s="11" t="s">
         <v>409</v>
@@ -7390,7 +7413,7 @@
       <c r="Q246" s="13"/>
       <c r="R246" s="14"/>
     </row>
-    <row r="247" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A247" s="13"/>
       <c r="B247" s="11" t="s">
         <v>410</v>
@@ -7404,7 +7427,7 @@
       <c r="Q247" s="13"/>
       <c r="R247" s="14"/>
     </row>
-    <row r="248" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A248" s="13"/>
       <c r="B248" s="11" t="s">
         <v>411</v>
@@ -7418,7 +7441,7 @@
       <c r="Q248" s="13"/>
       <c r="R248" s="14"/>
     </row>
-    <row r="249" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A249" s="13"/>
       <c r="B249" s="11" t="s">
         <v>412</v>
@@ -7432,7 +7455,7 @@
       <c r="Q249" s="13"/>
       <c r="R249" s="14"/>
     </row>
-    <row r="250" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A250" s="13"/>
       <c r="B250" s="11" t="s">
         <v>413</v>
@@ -7452,7 +7475,7 @@
       <c r="Q250" s="13"/>
       <c r="R250" s="14"/>
     </row>
-    <row r="251" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A251" s="13"/>
       <c r="B251" s="12" t="s">
         <v>83</v>
@@ -7484,7 +7507,7 @@
       <c r="Q251" s="13"/>
       <c r="R251" s="14"/>
     </row>
-    <row r="252" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A252" s="13"/>
       <c r="B252" s="11" t="s">
         <v>416</v>
@@ -7498,7 +7521,7 @@
       <c r="Q252" s="13"/>
       <c r="R252" s="14"/>
     </row>
-    <row r="253" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A253" s="13"/>
       <c r="B253" s="16" t="s">
         <v>238</v>
@@ -7527,7 +7550,7 @@
       <c r="Q253" s="13"/>
       <c r="R253" s="14"/>
     </row>
-    <row r="254" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A254" s="13"/>
       <c r="B254" s="11" t="s">
         <v>417</v>
@@ -7541,7 +7564,7 @@
       <c r="Q254" s="12"/>
       <c r="R254" s="14"/>
     </row>
-    <row r="255" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B255" s="16" t="s">
         <v>291</v>
       </c>
@@ -7568,7 +7591,7 @@
       </c>
       <c r="Q255" s="13"/>
     </row>
-    <row r="256" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A256" s="13"/>
       <c r="B256" s="12" t="s">
         <v>76</v>
@@ -7591,7 +7614,7 @@
       <c r="P256" s="12"/>
       <c r="R256" s="14"/>
     </row>
-    <row r="257" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A257" s="12"/>
       <c r="B257" s="11" t="s">
         <v>418</v>
@@ -7604,7 +7627,7 @@
       </c>
       <c r="R257" s="12"/>
     </row>
-    <row r="258" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B258" s="11" t="s">
         <v>419</v>
       </c>
@@ -7615,7 +7638,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="259" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A259" s="13"/>
       <c r="B259" s="11" t="s">
         <v>420</v>
@@ -7628,7 +7651,7 @@
       </c>
       <c r="R259" s="14"/>
     </row>
-    <row r="260" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A260" s="13"/>
       <c r="B260" s="11" t="s">
         <v>421</v>
@@ -7642,7 +7665,7 @@
       <c r="Q260" s="12"/>
       <c r="R260" s="14"/>
     </row>
-    <row r="261" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B261" s="11" t="s">
         <v>422</v>
       </c>
@@ -7654,7 +7677,7 @@
       </c>
       <c r="Q261" s="13"/>
     </row>
-    <row r="262" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A262" s="12"/>
       <c r="B262" s="11" t="s">
         <v>423</v>
@@ -7668,7 +7691,7 @@
       <c r="Q262" s="13"/>
       <c r="R262" s="12"/>
     </row>
-    <row r="263" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B263" s="11" t="s">
         <v>424</v>
       </c>
@@ -7679,7 +7702,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="264" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A264" s="13"/>
       <c r="B264" s="13" t="s">
         <v>246</v>
@@ -7692,7 +7715,7 @@
       </c>
       <c r="R264" s="14"/>
     </row>
-    <row r="265" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B265" s="16" t="s">
         <v>476</v>
       </c>
@@ -7719,7 +7742,7 @@
       </c>
       <c r="Q265" s="13"/>
     </row>
-    <row r="266" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B266" s="11" t="s">
         <v>426</v>
       </c>
@@ -7730,7 +7753,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="267" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B267" s="11" t="s">
         <v>427</v>
       </c>
@@ -7741,7 +7764,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="268" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A268" s="13"/>
       <c r="B268" s="11" t="s">
         <v>428</v>
@@ -7754,7 +7777,7 @@
       </c>
       <c r="R268" s="14"/>
     </row>
-    <row r="269" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B269" s="11" t="s">
         <v>429</v>
       </c>
@@ -7765,7 +7788,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="270" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B270" s="11" t="s">
         <v>430</v>
       </c>
@@ -7777,7 +7800,7 @@
       </c>
       <c r="Q270" s="13"/>
     </row>
-    <row r="271" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B271" s="11" t="s">
         <v>431</v>
       </c>
@@ -7788,7 +7811,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="272" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B272" s="11" t="s">
         <v>432</v>
       </c>
@@ -7799,7 +7822,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="273" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B273" s="11" t="s">
         <v>433</v>
       </c>
@@ -7810,7 +7833,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="274" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A274" s="13"/>
       <c r="B274" s="11" t="s">
         <v>434</v>
@@ -7824,7 +7847,7 @@
       <c r="Q274" s="13"/>
       <c r="R274" s="14"/>
     </row>
-    <row r="275" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A275" s="13"/>
       <c r="B275" s="11" t="s">
         <v>435</v>
@@ -7837,7 +7860,7 @@
       </c>
       <c r="R275" s="14"/>
     </row>
-    <row r="276" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A276" s="13"/>
       <c r="B276" s="11" t="s">
         <v>436</v>
@@ -7850,7 +7873,7 @@
       </c>
       <c r="R276" s="14"/>
     </row>
-    <row r="277" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B277" s="11" t="s">
         <v>437</v>
       </c>
@@ -7862,7 +7885,7 @@
       </c>
       <c r="Q277" s="13"/>
     </row>
-    <row r="278" spans="1:19" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B278" s="11" t="s">
         <v>438</v>
       </c>
@@ -7874,7 +7897,7 @@
       </c>
       <c r="Q278" s="13"/>
     </row>
-    <row r="279" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B279" s="11" t="s">
         <v>439</v>
       </c>
@@ -7886,7 +7909,7 @@
       </c>
       <c r="Q279" s="13"/>
     </row>
-    <row r="280" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A280" s="13"/>
       <c r="B280" s="11" t="s">
         <v>440</v>
@@ -7899,7 +7922,7 @@
       </c>
       <c r="R280" s="14"/>
     </row>
-    <row r="281" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:19" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A281" s="13"/>
       <c r="B281" s="11" t="s">
         <v>441</v>
@@ -7912,7 +7935,7 @@
       </c>
       <c r="R281" s="14"/>
     </row>
-    <row r="282" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A282" s="13"/>
       <c r="B282" s="11" t="s">
         <v>442</v>
@@ -7925,7 +7948,7 @@
       </c>
       <c r="R282" s="14"/>
     </row>
-    <row r="283" spans="1:19" s="19" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A283" s="11"/>
       <c r="B283" s="11" t="s">
         <v>443</v>
@@ -7952,7 +7975,7 @@
       <c r="R283" s="11"/>
       <c r="S283" s="11"/>
     </row>
-    <row r="284" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B284" s="11" t="s">
         <v>444</v>
       </c>
@@ -7963,7 +7986,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="285" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B285" s="11" t="s">
         <v>445</v>
       </c>
@@ -7974,7 +7997,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="286" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A286" s="13"/>
       <c r="B286" s="11" t="s">
         <v>446</v>
@@ -7987,7 +8010,7 @@
       </c>
       <c r="R286" s="14"/>
     </row>
-    <row r="287" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B287" s="11" t="s">
         <v>447</v>
       </c>
@@ -7998,7 +8021,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="288" spans="1:19" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B288" s="11" t="s">
         <v>448</v>
       </c>
@@ -8009,7 +8032,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="289" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B289" s="11" t="s">
         <v>449</v>
       </c>
@@ -8020,7 +8043,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="290" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B290" s="11" t="s">
         <v>450</v>
       </c>
@@ -8032,7 +8055,7 @@
       </c>
       <c r="Q290" s="13"/>
     </row>
-    <row r="291" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B291" s="11" t="s">
         <v>451</v>
       </c>
@@ -8044,7 +8067,7 @@
       </c>
       <c r="Q291" s="13"/>
     </row>
-    <row r="292" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B292" s="11" t="s">
         <v>506</v>
       </c>
@@ -8052,7 +8075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B293" s="11" t="s">
         <v>452</v>
       </c>
@@ -8063,7 +8086,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="294" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A294" s="13"/>
       <c r="B294" s="11" t="s">
         <v>453</v>
@@ -8077,7 +8100,7 @@
       <c r="Q294" s="13"/>
       <c r="R294" s="14"/>
     </row>
-    <row r="295" spans="1:18" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:18" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B295" s="16" t="s">
         <v>293</v>
       </c>
@@ -8103,7 +8126,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="296" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B296" s="11" t="s">
         <v>454</v>
       </c>
@@ -8115,7 +8138,7 @@
       </c>
       <c r="Q296" s="13"/>
     </row>
-    <row r="297" spans="1:18" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:18" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B297" s="12" t="s">
         <v>70</v>
       </c>
@@ -8143,7 +8166,7 @@
       <c r="P297" s="12"/>
       <c r="Q297" s="13"/>
     </row>
-    <row r="298" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A298" s="13"/>
       <c r="B298" s="11" t="s">
         <v>455</v>
@@ -8157,7 +8180,7 @@
       <c r="Q298" s="13"/>
       <c r="R298" s="14"/>
     </row>
-    <row r="299" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A299" s="13"/>
       <c r="B299" s="11" t="s">
         <v>456</v>
@@ -8171,7 +8194,7 @@
       <c r="Q299" s="13"/>
       <c r="R299" s="14"/>
     </row>
-    <row r="300" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A300" s="13"/>
       <c r="B300" s="11" t="s">
         <v>457</v>
@@ -8185,7 +8208,7 @@
       <c r="Q300" s="13"/>
       <c r="R300" s="14"/>
     </row>
-    <row r="301" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A301" s="13"/>
       <c r="B301" s="11" t="s">
         <v>458</v>
@@ -8198,7 +8221,7 @@
       </c>
       <c r="R301" s="14"/>
     </row>
-    <row r="302" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A302" s="13"/>
       <c r="B302" s="11" t="s">
         <v>459</v>
@@ -8211,7 +8234,7 @@
       </c>
       <c r="R302" s="14"/>
     </row>
-    <row r="303" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A303" s="13"/>
       <c r="B303" s="11" t="s">
         <v>460</v>
@@ -8224,7 +8247,7 @@
       </c>
       <c r="R303" s="14"/>
     </row>
-    <row r="304" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B304" s="11" t="s">
         <v>461</v>
       </c>
@@ -8236,7 +8259,7 @@
       </c>
       <c r="Q304" s="12"/>
     </row>
-    <row r="305" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B305" s="11" t="s">
         <v>462</v>
       </c>
@@ -8247,7 +8270,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="306" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B306" s="11" t="s">
         <v>463</v>
       </c>
@@ -8258,7 +8281,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="307" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A307" s="12" t="s">
         <v>71</v>
       </c>
@@ -8273,7 +8296,7 @@
       </c>
       <c r="R307" s="12"/>
     </row>
-    <row r="308" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:20" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A308" s="12"/>
       <c r="B308" s="11" t="s">
         <v>522</v>
@@ -8292,7 +8315,7 @@
       </c>
       <c r="R308" s="12"/>
     </row>
-    <row r="309" spans="1:20" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B309" s="17" t="s">
         <v>526</v>
       </c>
@@ -8311,7 +8334,7 @@
       </c>
       <c r="T309" s="15"/>
     </row>
-    <row r="310" spans="1:20" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B310" s="17" t="s">
         <v>528</v>
       </c>
@@ -8330,7 +8353,7 @@
       </c>
       <c r="T310" s="15"/>
     </row>
-    <row r="311" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B311" s="11" t="s">
         <v>465</v>
       </c>
@@ -8341,7 +8364,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="312" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B312" s="13" t="s">
         <v>269</v>
       </c>
@@ -8352,7 +8375,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="313" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B313" s="13" t="s">
         <v>270</v>
       </c>
@@ -8363,7 +8386,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="314" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B314" s="13" t="s">
         <v>272</v>
       </c>
@@ -8377,7 +8400,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="315" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B315" s="11" t="s">
         <v>469</v>
       </c>
@@ -8388,7 +8411,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="316" spans="1:20" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:20" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B316" s="11" t="s">
         <v>470</v>
       </c>
@@ -8399,7 +8422,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="317" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:20" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B317" s="11" t="s">
         <v>471</v>
       </c>
@@ -8411,13 +8434,13 @@
       </c>
       <c r="Q317" s="13"/>
     </row>
-    <row r="318" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B318" s="14"/>
       <c r="P318" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="319" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B319" s="14"/>
       <c r="F319" s="12"/>
       <c r="G319" s="12"/>
@@ -8433,25 +8456,25 @@
       <c r="O319" s="12"/>
       <c r="P319" s="12"/>
     </row>
-    <row r="320" spans="1:20" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B320" s="14"/>
       <c r="P320" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="321" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B321" s="14"/>
       <c r="P321" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="322" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B322" s="14"/>
       <c r="P322" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="323" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B323" s="14"/>
       <c r="D323" s="12"/>
       <c r="E323" s="12"/>
@@ -8467,13 +8490,13 @@
       <c r="O323" s="12"/>
       <c r="P323" s="12"/>
     </row>
-    <row r="324" spans="1:18" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B324" s="14"/>
       <c r="P324" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="325" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B325" s="14"/>
       <c r="C325" s="12"/>
       <c r="D325" s="12"/>
@@ -8490,7 +8513,7 @@
       <c r="O325" s="12"/>
       <c r="P325" s="12"/>
     </row>
-    <row r="326" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B326" s="14"/>
       <c r="C326" s="12"/>
       <c r="D326" s="12"/>
@@ -8507,44 +8530,44 @@
       <c r="O326" s="12"/>
       <c r="P326" s="12"/>
     </row>
-    <row r="327" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B327" s="14"/>
       <c r="Q327" s="12"/>
     </row>
-    <row r="328" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B328" s="14"/>
     </row>
-    <row r="329" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B329" s="14"/>
     </row>
-    <row r="330" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B330" s="14"/>
     </row>
-    <row r="331" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B331" s="14"/>
     </row>
-    <row r="332" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B332" s="14"/>
     </row>
-    <row r="333" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B333" s="14"/>
     </row>
-    <row r="334" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B334" s="14"/>
     </row>
-    <row r="335" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B335" s="14"/>
     </row>
-    <row r="336" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A336" s="14"/>
       <c r="B336" s="14"/>
       <c r="R336" s="12"/>
     </row>
-    <row r="337" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B337" s="14"/>
       <c r="Q337" s="12"/>
     </row>
-    <row r="338" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B338" s="14"/>
       <c r="C338" s="12"/>
       <c r="D338" s="12"/>
@@ -8561,7 +8584,7 @@
       <c r="O338" s="12"/>
       <c r="P338" s="12"/>
     </row>
-    <row r="339" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B339" s="14"/>
       <c r="C339" s="12"/>
       <c r="D339" s="12"/>
@@ -8579,7 +8602,7 @@
       <c r="P339" s="12"/>
       <c r="Q339" s="12"/>
     </row>
-    <row r="340" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A340" s="12"/>
       <c r="B340" s="14"/>
       <c r="C340" s="12"/>
@@ -8599,7 +8622,7 @@
       <c r="Q340" s="12"/>
       <c r="R340" s="12"/>
     </row>
-    <row r="341" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B341" s="14"/>
       <c r="C341" s="12"/>
       <c r="D341" s="12"/>
@@ -8617,11 +8640,11 @@
       <c r="P341" s="12"/>
       <c r="Q341" s="12"/>
     </row>
-    <row r="342" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B342" s="14"/>
     </row>
   </sheetData>
-  <sortState ref="A2:S2824">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S2824">
     <sortCondition ref="F2:F2824"/>
     <sortCondition descending="1" ref="N2:N2824"/>
     <sortCondition ref="B2:B2824"/>
@@ -8642,16 +8665,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="4" customWidth="1"/>
     <col min="3" max="3" width="93" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.1640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="4"/>
+    <col min="4" max="4" width="45.1796875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>104</v>
       </c>
@@ -8665,7 +8688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -8676,7 +8699,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -8687,7 +8710,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -8701,7 +8724,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
@@ -8712,7 +8735,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -8726,7 +8749,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>103</v>
       </c>
@@ -8737,7 +8760,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>88</v>
       </c>
@@ -8748,7 +8771,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>87</v>
       </c>
@@ -8759,7 +8782,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -8770,7 +8793,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
@@ -8781,7 +8804,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>86</v>
       </c>
@@ -8792,7 +8815,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -8803,7 +8826,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>99</v>
       </c>
@@ -8814,7 +8837,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>150</v>
       </c>
@@ -8825,7 +8848,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>151</v>
       </c>
@@ -8836,7 +8859,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>152</v>
       </c>
@@ -8847,7 +8870,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>153</v>
       </c>
@@ -8858,7 +8881,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>495</v>
       </c>
@@ -8883,22 +8906,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="36.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="14.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.36328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="36.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.36328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.36328125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -8936,7 +8959,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -8950,7 +8973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -8964,7 +8987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -8981,7 +9004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -8992,7 +9015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -9006,7 +9029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -9023,7 +9046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -9037,7 +9060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
@@ -9054,7 +9077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -9081,7 +9104,7 @@
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9096,12 +9119,12 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="43.33203125" customWidth="1"/>
+    <col min="11" max="11" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -9136,7 +9159,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9147,7 +9170,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9164,7 +9187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9181,7 +9204,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9198,7 +9221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9215,7 +9238,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9232,7 +9255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9249,7 +9272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9266,7 +9289,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9283,7 +9306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9300,7 +9323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9326,7 +9349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9352,7 +9375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9378,7 +9401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9404,7 +9427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9430,7 +9453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9456,7 +9479,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9482,7 +9505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9508,7 +9531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9534,7 +9557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9560,7 +9583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9586,7 +9609,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9612,7 +9635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9638,7 +9661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9664,7 +9687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9690,7 +9713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9716,7 +9739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9742,7 +9765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9768,7 +9791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>

</xml_diff>